<commit_message>
Updates to - Algorithms to Live By - How to Build a Brain - Principles of Computational Modelling in Neuroscience
</commit_message>
<xml_diff>
--- a/Algorithms to Live By.xlsx
+++ b/Algorithms to Live By.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="465" windowWidth="27555" windowHeight="12240" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="465" windowWidth="27555" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -290,6 +290,15 @@
                 <c:pt idx="10">
                   <c:v>12.614965986346409</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.640763462958686</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.666666666934775</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.153846153745317</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -350,6 +359,15 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>13.27450623620086</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.307376962101211</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.564591384339288</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.707930306809725</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -805,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1128,7 @@
         <v>0.80327868852765616</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" ref="H8" si="23">G8*60</f>
+        <f>G8*60</f>
         <v>48.196721311659367</v>
       </c>
       <c r="I8" s="2">
@@ -1136,19 +1154,19 @@
         <v>364</v>
       </c>
       <c r="E9" s="11">
-        <f t="shared" ref="E9" si="24">C9-A9</f>
+        <f t="shared" ref="E9" si="23">C9-A9</f>
         <v>4.0277777778101154E-2</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9" si="25">D9-B9+1</f>
+        <f t="shared" ref="F9" si="24">D9-B9+1</f>
         <v>49</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" ref="G9" si="26">F9/(E9*24*60)</f>
+        <f t="shared" ref="G9" si="25">F9/(E9*24*60)</f>
         <v>0.84482758620011378</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" ref="H9" si="27">G9*60</f>
+        <f t="shared" ref="H9" si="26">G9*60</f>
         <v>50.689655172006823</v>
       </c>
       <c r="I9" s="2">
@@ -1174,19 +1192,19 @@
         <v>398</v>
       </c>
       <c r="E10" s="11">
-        <f t="shared" ref="E10" si="28">C10-A10</f>
+        <f t="shared" ref="E10" si="27">C10-A10</f>
         <v>4.0277777778101154E-2</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10" si="29">D10-B10+1</f>
+        <f t="shared" ref="F10" si="28">D10-B10+1</f>
         <v>34</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" ref="G10" si="30">F10/(E10*24*60)</f>
+        <f t="shared" ref="G10" si="29">F10/(E10*24*60)</f>
         <v>0.58620689654701774</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" ref="H10" si="31">G10*60</f>
+        <f t="shared" ref="H10" si="30">G10*60</f>
         <v>35.172413792821061</v>
       </c>
       <c r="I10" s="2">
@@ -1212,19 +1230,19 @@
         <v>442</v>
       </c>
       <c r="E11" s="11">
-        <f t="shared" ref="E11" si="32">C11-A11</f>
+        <f t="shared" ref="E11" si="31">C11-A11</f>
         <v>4.3055555550381541E-2</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11" si="33">D11-B11+1</f>
+        <f t="shared" ref="F11" si="32">D11-B11+1</f>
         <v>44</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" ref="G11" si="34">F11/(E11*24*60)</f>
+        <f t="shared" ref="G11" si="33">F11/(E11*24*60)</f>
         <v>0.70967741944012108</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" ref="H11" si="35">G11*60</f>
+        <f t="shared" ref="H11" si="34">G11*60</f>
         <v>42.580645166407265</v>
       </c>
       <c r="I11" s="2">
@@ -1250,19 +1268,19 @@
         <v>489</v>
       </c>
       <c r="E12" s="11">
-        <f t="shared" ref="E12" si="36">C12-A12</f>
+        <f t="shared" ref="E12" si="35">C12-A12</f>
         <v>3.8194444445252884E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12" si="37">D12-B12+1</f>
+        <f t="shared" ref="F12" si="36">D12-B12+1</f>
         <v>47</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" ref="G12" si="38">F12/(E12*24*60)</f>
+        <f t="shared" ref="G12" si="37">F12/(E12*24*60)</f>
         <v>0.85454545452736685</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" ref="H12" si="39">G12*60</f>
+        <f t="shared" ref="H12" si="38">G12*60</f>
         <v>51.272727271642012</v>
       </c>
       <c r="I12" s="2">
@@ -1275,28 +1293,118 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="A13" s="12">
+        <v>42965.958333333336</v>
+      </c>
+      <c r="B13">
+        <v>490</v>
+      </c>
+      <c r="C13" s="12">
+        <v>42965.995833333334</v>
+      </c>
+      <c r="D13">
+        <v>529</v>
+      </c>
+      <c r="E13" s="11">
+        <f t="shared" ref="E13" si="39">C13-A13</f>
+        <v>3.7499999998544808E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13" si="40">D13-B13+1</f>
+        <v>40</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" ref="G13" si="41">F13/(E13*24*60)</f>
+        <v>0.74074074076948526</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" ref="H13" si="42">G13*60</f>
+        <v>44.444444446169115</v>
+      </c>
+      <c r="I13" s="2">
+        <f>Sheet2!$B$25/MEDIAN($H$2:H13)</f>
+        <v>12.640763462958686</v>
+      </c>
+      <c r="J13" s="2">
+        <f>Sheet2!$B$25/AVERAGE($H$2:H13)</f>
+        <v>13.307376962101211</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="10"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="A14" s="12">
+        <v>42966.950694444444</v>
+      </c>
+      <c r="B14">
+        <v>530</v>
+      </c>
+      <c r="C14" s="12">
+        <v>42966.993055555555</v>
+      </c>
+      <c r="D14">
+        <v>564</v>
+      </c>
+      <c r="E14" s="11">
+        <f t="shared" ref="E14" si="43">C14-A14</f>
+        <v>4.2361111110949423E-2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14" si="44">D14-B14+1</f>
+        <v>35</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" ref="G14" si="45">F14/(E14*24*60)</f>
+        <v>0.57377049180546869</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" ref="H14" si="46">G14*60</f>
+        <v>34.42622950832812</v>
+      </c>
+      <c r="I14" s="2">
+        <f>Sheet2!$B$25/MEDIAN($H$2:H14)</f>
+        <v>12.666666666934775</v>
+      </c>
+      <c r="J14" s="2">
+        <f>Sheet2!$B$25/AVERAGE($H$2:H14)</f>
+        <v>13.564591384339288</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="10"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="A15" s="12">
+        <v>42971.691666666666</v>
+      </c>
+      <c r="B15">
+        <v>565</v>
+      </c>
+      <c r="C15" s="12">
+        <v>42971.739583333336</v>
+      </c>
+      <c r="D15">
+        <v>608</v>
+      </c>
+      <c r="E15" s="11">
+        <f t="shared" ref="E15" si="47">C15-A15</f>
+        <v>4.7916666670062114E-2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F15" si="48">D15-B15+1</f>
+        <v>44</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" ref="G15" si="49">F15/(E15*24*60)</f>
+        <v>0.63768115937510284</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" ref="H15" si="50">G15*60</f>
+        <v>38.260869562506173</v>
+      </c>
+      <c r="I15" s="2">
+        <f>Sheet2!$B$25/MEDIAN($H$2:H15)</f>
+        <v>13.153846153745317</v>
+      </c>
+      <c r="J15" s="2">
+        <f>Sheet2!$B$25/AVERAGE($H$2:H15)</f>
+        <v>13.707930306809725</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
@@ -2074,7 +2182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A25:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -2097,7 +2205,7 @@
       </c>
       <c r="B26">
         <f>MAX(Sheet1!D2:D1000)</f>
-        <v>489</v>
+        <v>608</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2106,7 +2214,7 @@
       </c>
       <c r="B27" s="4">
         <f>B26/B25*100</f>
-        <v>80.42763157894737</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2115,7 +2223,7 @@
       </c>
       <c r="B28">
         <f>B25-B26</f>
-        <v>119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2124,7 +2232,7 @@
       </c>
       <c r="B29" s="4">
         <f>B28/B25*100</f>
-        <v>19.572368421052634</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2133,7 +2241,7 @@
       </c>
       <c r="B30" s="4">
         <f>B25/H38</f>
-        <v>12.614965986346409</v>
+        <v>13.153846153745317</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2142,7 +2250,7 @@
       </c>
       <c r="B31" s="4">
         <f>B25/H39</f>
-        <v>13.27450623620086</v>
+        <v>13.707930306809725</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2151,7 +2259,7 @@
       </c>
       <c r="B32" s="2">
         <f>ABS(B30-B31)</f>
-        <v>0.65954024985445159</v>
+        <v>0.55408415306440872</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2160,7 +2268,7 @@
       </c>
       <c r="B33" s="2">
         <f>B28/H38</f>
-        <v>2.4690476190381951</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2169,7 +2277,7 @@
       </c>
       <c r="B34" s="2">
         <f>B28/H39</f>
-        <v>2.5981352666248396</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2213,7 +2321,7 @@
       </c>
       <c r="E37" s="11">
         <f>MAX(Sheet1!E2:E1000)</f>
-        <v>4.3055555550381541E-2</v>
+        <v>4.7916666670062114E-2</v>
       </c>
       <c r="F37" s="4">
         <f>MAX(Sheet1!F2:F1000)</f>
@@ -2238,15 +2346,15 @@
       </c>
       <c r="F38" s="4">
         <f>MEDIAN(Sheet1!F2:F1000)</f>
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G38" s="4">
         <f>MEDIAN(Sheet1!G2:G1000)</f>
-        <v>0.80327868852765616</v>
+        <v>0.77037037037627609</v>
       </c>
       <c r="H38" s="4">
         <f>MEDIAN(Sheet1!H2:H1000)</f>
-        <v>48.196721311659367</v>
+        <v>46.222222222576562</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2255,19 +2363,19 @@
       </c>
       <c r="E39" s="11">
         <f>AVERAGE(Sheet1!E2:E1000)</f>
-        <v>4.008838383742841E-2</v>
+        <v>4.0624999999376347E-2</v>
       </c>
       <c r="F39" s="4">
         <f>AVERAGE(Sheet1!F2:F1000)</f>
-        <v>44</v>
+        <v>43.071428571428569</v>
       </c>
       <c r="G39" s="4">
         <f>AVERAGE(Sheet1!G2:G1000)</f>
-        <v>0.76336800428017071</v>
+        <v>0.73923145993085249</v>
       </c>
       <c r="H39" s="4">
         <f>AVERAGE(Sheet1!H2:H1000)</f>
-        <v>45.80208025681025</v>
+        <v>44.353887595851155</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2276,11 +2384,11 @@
       </c>
       <c r="E40" s="3" t="str">
         <f>TEXT(SUM(Sheet1!E2:E1000), "d:h:mm:ss")</f>
-        <v>0:10:35:00</v>
+        <v>0:13:39:00</v>
       </c>
       <c r="F40" s="4">
         <f>SUM(Sheet1!F2:F1000)</f>
-        <v>484</v>
+        <v>603</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>

</xml_diff>